<commit_message>
update solidity test step
</commit_message>
<xml_diff>
--- a/交易所场景CheckList/交易所场景CheckList.xlsx
+++ b/交易所场景CheckList/交易所场景CheckList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
   <si>
     <t>版本：</t>
   </si>
@@ -202,9 +202,6 @@
     <t>买的数量&lt;卖的数量:</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>委托价格=当前卖1价：成交</t>
   </si>
   <si>
@@ -213,11 +210,6 @@
 买的数量&lt;卖的数量:</t>
   </si>
   <si>
-    <t>1.OK
-2.OK
-3.OK</t>
-  </si>
-  <si>
     <t>委托价格&lt;当前卖1价：不成交</t>
   </si>
   <si>
@@ -249,9 +241,6 @@
   </si>
   <si>
     <t>委托价格&lt;当前买1价：按买价成交</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
   <si>
     <t>委托价格=当前买1价：成交</t>
@@ -355,6 +344,11 @@
   <si>
     <t>卖方</t>
   </si>
+  <si>
+    <t>动态撮合
+()</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -363,7 +357,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +406,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="5">
@@ -571,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -609,51 +610,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -680,6 +636,54 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,11 +986,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z289"/>
+  <dimension ref="A1:Z290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1002,11 +1006,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1032,11 +1036,11 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1062,11 +1066,11 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1089,13 +1093,13 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1336,7 +1340,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1431,7 +1435,7 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A15" s="13"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1460,7 +1464,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="38.25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>21</v>
@@ -1490,7 +1494,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
@@ -1522,8 +1526,8 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A18" s="22"/>
       <c r="B18" s="4" t="s">
         <v>24</v>
       </c>
@@ -1552,8 +1556,8 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A19" s="13"/>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A19" s="22"/>
       <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
@@ -1583,7 +1587,7 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A20" s="13"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
@@ -1612,7 +1616,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A21" s="12"/>
       <c r="B21" s="4" t="s">
         <v>27</v>
@@ -1642,7 +1646,7 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
         <v>28</v>
       </c>
@@ -1675,7 +1679,7 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A23" s="13"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="4" t="s">
         <v>30</v>
       </c>
@@ -1705,7 +1709,7 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A24" s="13"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
@@ -1735,7 +1739,7 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A25" s="13"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="4" t="s">
         <v>32</v>
       </c>
@@ -1765,7 +1769,7 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A26" s="13"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="4" t="s">
         <v>33</v>
       </c>
@@ -1795,7 +1799,7 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A27" s="13"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="4" t="s">
         <v>34</v>
       </c>
@@ -1825,7 +1829,7 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A28" s="13"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="4" t="s">
         <v>35</v>
       </c>
@@ -1855,7 +1859,7 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A29" s="13"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
@@ -1885,7 +1889,7 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A30" s="13"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>37</v>
       </c>
@@ -1944,7 +1948,7 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" spans="1:26" ht="63.75" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:26" ht="51" x14ac:dyDescent="0.15">
       <c r="A32" s="11" t="s">
         <v>39</v>
       </c>
@@ -1976,8 +1980,8 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
     </row>
-    <row r="33" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A33" s="13"/>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>41</v>
       </c>
@@ -2006,8 +2010,8 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A34" s="22"/>
       <c r="B34" s="4" t="s">
         <v>42</v>
       </c>
@@ -2036,8 +2040,8 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A35" s="13"/>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A35" s="22"/>
       <c r="B35" s="4" t="s">
         <v>43</v>
       </c>
@@ -2067,7 +2071,7 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A36" s="13"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="11" t="s">
         <v>44</v>
       </c>
@@ -2128,7 +2132,7 @@
       <c r="A38" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -2159,8 +2163,8 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A39" s="13"/>
-      <c r="B39" s="23"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="4" t="s">
         <v>48</v>
       </c>
@@ -2189,8 +2193,8 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A40" s="13"/>
-      <c r="B40" s="23"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="4" t="s">
         <v>49</v>
       </c>
@@ -2219,8 +2223,8 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A41" s="13"/>
-      <c r="B41" s="23"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="4" t="s">
         <v>50</v>
       </c>
@@ -2249,8 +2253,8 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A42" s="13"/>
-      <c r="B42" s="23"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="4" t="s">
         <v>51</v>
       </c>
@@ -2279,13 +2283,13 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A43" s="13"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="14" t="s">
+      <c r="A43" s="22"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="16"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="24"/>
       <c r="F43" s="5" t="s">
         <v>53</v>
       </c>
@@ -2311,15 +2315,15 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="13"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="17" t="s">
+      <c r="A44" s="22"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="16"/>
+      <c r="E44" s="24"/>
       <c r="F44" s="6"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2343,16 +2347,16 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="13"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="17" t="s">
+      <c r="A45" s="22"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="20"/>
+      <c r="F45" s="35"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -2375,12 +2379,12 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A46" s="13"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="12"/>
-      <c r="F46" s="21"/>
+      <c r="F46" s="36"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -2403,14 +2407,14 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A47" s="13"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F47" s="20"/>
+      <c r="F47" s="35"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -2433,12 +2437,12 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A48" s="13"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="12"/>
-      <c r="F48" s="21"/>
+      <c r="F48" s="36"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -2461,16 +2465,14 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A49" s="13"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F49" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="F49" s="11"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -2493,10 +2495,10 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A50" s="13"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="19"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="31"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="2"/>
@@ -2521,13 +2523,13 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="13"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" s="16"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="24"/>
       <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2551,18 +2553,16 @@
       <c r="Z51" s="2"/>
     </row>
     <row r="52" spans="1:26" ht="38.25" x14ac:dyDescent="0.15">
-      <c r="A52" s="13"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="30"/>
       <c r="D52" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -2585,13 +2585,13 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="13"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E53" s="16"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="24"/>
       <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -2615,18 +2615,16 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A54" s="13"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="19"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="31"/>
       <c r="D54" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F54" s="4"/>
       <c r="G54" s="6"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -2649,10 +2647,10 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A55" s="13"/>
-      <c r="B55" s="23"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -2679,16 +2677,14 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A56" s="13"/>
-      <c r="B56" s="23"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="8"/>
-      <c r="F56" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -2711,8 +2707,8 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A57" s="13"/>
-      <c r="B57" s="23"/>
+      <c r="A57" s="22"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -2739,10 +2735,10 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A58" s="13"/>
-      <c r="B58" s="23"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -2769,16 +2765,14 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A59" s="13"/>
-      <c r="B59" s="23"/>
+      <c r="A59" s="22"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2801,8 +2795,8 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A60" s="13"/>
-      <c r="B60" s="24"/>
+      <c r="A60" s="22"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -2829,17 +2823,17 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A61" s="13"/>
-      <c r="B61" s="25" t="s">
+      <c r="A61" s="22"/>
+      <c r="B61" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" s="28"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -2863,15 +2857,15 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="13"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="17" t="s">
+      <c r="A62" s="22"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D62" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E62" s="16"/>
+      <c r="D62" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E62" s="24"/>
       <c r="F62" s="6"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -2895,18 +2889,16 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A63" s="13"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="17" t="s">
+      <c r="A63" s="22"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -2929,16 +2921,14 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A64" s="13"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
       <c r="E64" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F64" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2961,16 +2951,14 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A65" s="13"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="19"/>
+      <c r="A65" s="22"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="31"/>
       <c r="E65" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F65" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -2993,11 +2981,11 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A66" s="13"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="22"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="30"/>
       <c r="D66" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="4"/>
@@ -3023,14 +3011,14 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67" spans="1:26" ht="38.25" x14ac:dyDescent="0.15">
-      <c r="A67" s="13"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="18"/>
+      <c r="A67" s="22"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="30"/>
       <c r="D67" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="2"/>
@@ -3055,13 +3043,13 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="13"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E68" s="16"/>
+      <c r="A68" s="22"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E68" s="24"/>
       <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -3085,18 +3073,16 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A69" s="13"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="19"/>
+      <c r="A69" s="22"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="31"/>
       <c r="D69" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -3119,10 +3105,10 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A70" s="13"/>
-      <c r="B70" s="26"/>
+      <c r="A70" s="22"/>
+      <c r="B70" s="33"/>
       <c r="C70" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -3149,16 +3135,14 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A71" s="13"/>
-      <c r="B71" s="26"/>
+      <c r="A71" s="22"/>
+      <c r="B71" s="33"/>
       <c r="C71" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="8"/>
-      <c r="F71" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -3181,8 +3165,8 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A72" s="13"/>
-      <c r="B72" s="26"/>
+      <c r="A72" s="22"/>
+      <c r="B72" s="33"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -3209,10 +3193,10 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A73" s="13"/>
-      <c r="B73" s="26"/>
+      <c r="A73" s="22"/>
+      <c r="B73" s="33"/>
       <c r="C73" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -3239,16 +3223,14 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A74" s="13"/>
-      <c r="B74" s="26"/>
+      <c r="A74" s="22"/>
+      <c r="B74" s="33"/>
       <c r="C74" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
-      <c r="F74" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -3271,8 +3253,8 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A75" s="13"/>
-      <c r="B75" s="27"/>
+      <c r="A75" s="22"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -3298,14 +3280,12 @@
       <c r="Y75" s="2"/>
       <c r="Z75" s="2"/>
     </row>
-    <row r="76" spans="1:26" ht="114.75" x14ac:dyDescent="0.15">
-      <c r="A76" s="13"/>
-      <c r="B76" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>81</v>
-      </c>
+    <row r="76" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="22"/>
+      <c r="B76" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -3330,13 +3310,13 @@
       <c r="Y76" s="2"/>
       <c r="Z76" s="2"/>
     </row>
-    <row r="77" spans="1:26" ht="89.25" x14ac:dyDescent="0.15">
-      <c r="A77" s="13"/>
+    <row r="77" spans="1:26" ht="114.75" x14ac:dyDescent="0.15">
+      <c r="A77" s="22"/>
       <c r="B77" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -3362,10 +3342,14 @@
       <c r="Y77" s="2"/>
       <c r="Z77" s="2"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A78" s="12"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
+    <row r="78" spans="1:26" ht="89.25" x14ac:dyDescent="0.15">
+      <c r="A78" s="22"/>
+      <c r="B78" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -3390,19 +3374,11 @@
       <c r="Y78" s="2"/>
       <c r="Z78" s="2"/>
     </row>
-    <row r="79" spans="1:26" ht="51" x14ac:dyDescent="0.15">
-      <c r="A79" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>87</v>
-      </c>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A79" s="12"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="2"/>
@@ -3426,19 +3402,21 @@
       <c r="Y79" s="2"/>
       <c r="Z79" s="2"/>
     </row>
-    <row r="80" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>90</v>
-      </c>
+    <row r="80" spans="1:26" ht="51" x14ac:dyDescent="0.15">
+      <c r="A80" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -3460,13 +3438,19 @@
       <c r="Y80" s="2"/>
       <c r="Z80" s="2"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="4"/>
+    <row r="81" spans="1:26" ht="25.5" x14ac:dyDescent="0.15">
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -3489,13 +3473,11 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="12"/>
       <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -3518,19 +3500,15 @@
       <c r="Y82" s="2"/>
       <c r="Z82" s="2"/>
     </row>
-    <row r="83" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>94</v>
-      </c>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -3552,13 +3530,19 @@
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="4"/>
+    <row r="84" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -3581,13 +3565,11 @@
       <c r="Z84" s="2"/>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E85" s="4"/>
+      <c r="A85" s="22"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
       <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -3610,14 +3592,12 @@
       <c r="Y85" s="2"/>
       <c r="Z85" s="2"/>
     </row>
-    <row r="86" spans="1:26" ht="63.75" x14ac:dyDescent="0.15">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="11" t="s">
-        <v>96</v>
-      </c>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A86" s="22"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="12"/>
       <c r="D86" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -3642,19 +3622,17 @@
       <c r="Y86" s="2"/>
       <c r="Z86" s="2"/>
     </row>
-    <row r="87" spans="1:26" ht="38.25" x14ac:dyDescent="0.15">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>100</v>
-      </c>
+    <row r="87" spans="1:26" ht="63.75" x14ac:dyDescent="0.15">
+      <c r="A87" s="22"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -3676,17 +3654,19 @@
       <c r="Y87" s="2"/>
       <c r="Z87" s="2"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="11" t="s">
-        <v>101</v>
+    <row r="88" spans="1:26" ht="38.25" x14ac:dyDescent="0.15">
+      <c r="A88" s="22"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F88" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -3709,12 +3689,14 @@
       <c r="Z88" s="2"/>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="12"/>
+      <c r="A89" s="22"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E89" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="2"/>
@@ -3739,13 +3721,13 @@
       <c r="Z89" s="2"/>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A90" s="13"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E90" s="4"/>
+      <c r="A90" s="22"/>
+      <c r="B90" s="22"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -3769,12 +3751,12 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A91" s="13"/>
-      <c r="B91" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
+      <c r="A91" s="22"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="2"/>
@@ -3799,8 +3781,10 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
+      <c r="A92" s="22"/>
+      <c r="B92" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -3827,8 +3811,8 @@
       <c r="Z92" s="2"/>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="12"/>
+      <c r="B93" s="12"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -8223,12 +8207,12 @@
       <c r="Z249" s="2"/>
     </row>
     <row r="250" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A250" s="2"/>
-      <c r="B250" s="2"/>
-      <c r="C250" s="2"/>
-      <c r="D250" s="2"/>
-      <c r="E250" s="2"/>
-      <c r="F250" s="2"/>
+      <c r="A250" s="4"/>
+      <c r="B250" s="4"/>
+      <c r="C250" s="4"/>
+      <c r="D250" s="4"/>
+      <c r="E250" s="4"/>
+      <c r="F250" s="4"/>
       <c r="G250" s="2"/>
       <c r="H250" s="2"/>
       <c r="I250" s="2"/>
@@ -9342,22 +9326,55 @@
       <c r="Y289" s="2"/>
       <c r="Z289" s="2"/>
     </row>
+    <row r="290" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A290" s="2"/>
+      <c r="B290" s="2"/>
+      <c r="C290" s="2"/>
+      <c r="D290" s="2"/>
+      <c r="E290" s="2"/>
+      <c r="F290" s="2"/>
+      <c r="G290" s="2"/>
+      <c r="H290" s="2"/>
+      <c r="I290" s="2"/>
+      <c r="J290" s="2"/>
+      <c r="K290" s="2"/>
+      <c r="L290" s="2"/>
+      <c r="M290" s="2"/>
+      <c r="N290" s="2"/>
+      <c r="O290" s="2"/>
+      <c r="P290" s="2"/>
+      <c r="Q290" s="2"/>
+      <c r="R290" s="2"/>
+      <c r="S290" s="2"/>
+      <c r="T290" s="2"/>
+      <c r="U290" s="2"/>
+      <c r="V290" s="2"/>
+      <c r="W290" s="2"/>
+      <c r="X290" s="2"/>
+      <c r="Y290" s="2"/>
+      <c r="Z290" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="A80:A93"/>
+    <mergeCell ref="B80:B91"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A38:A78"/>
+    <mergeCell ref="A38:A79"/>
     <mergeCell ref="B38:B60"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="C44:C54"/>
@@ -9367,26 +9384,21 @@
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="B61:B75"/>
     <mergeCell ref="A32:A37"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="A79:A92"/>
-    <mergeCell ref="B79:B90"/>
-    <mergeCell ref="C79:C85"/>
-    <mergeCell ref="D80:D82"/>
-    <mergeCell ref="E80:E81"/>
     <mergeCell ref="C61:E61"/>
     <mergeCell ref="C62:C69"/>
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="D63:D65"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="C86:C90"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>